<commit_message>
Further updates and additions
</commit_message>
<xml_diff>
--- a/Library.xlsx
+++ b/Library.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnsonjoh/Desktop/Work/2018/December/mkeR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnsonjoh/milwaukeer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE7273EF-81C8-4249-8D6A-B3ADC4E9620B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4C755DB7-AAF6-514C-A648-5462399C3900}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22120" yWindow="3380" windowWidth="28040" windowHeight="17440" xr2:uid="{DE90C8FF-EFC0-B746-9E3E-CBBA0E7E6D7E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="70">
   <si>
     <t>Dataset</t>
   </si>
@@ -54,9 +54,6 @@
     <t>time</t>
   </si>
   <si>
-    <t>get_WIBRS</t>
-  </si>
-  <si>
     <t>87843297-a6fa-46d4-ba5d-cb342fb2d3bb</t>
   </si>
   <si>
@@ -75,12 +72,6 @@
     <t>property</t>
   </si>
   <si>
-    <t>get_MPROP</t>
-  </si>
-  <si>
-    <t>0a2c7f31-cd15-4151-8222-09dd57d5f16d</t>
-  </si>
-  <si>
     <t>Polling Places</t>
   </si>
   <si>
@@ -129,9 +120,6 @@
     <t>get_EMS</t>
   </si>
   <si>
-    <t>662070a0-eadc-4328-b0f5-e8e73531c8e2</t>
-  </si>
-  <si>
     <t>highest_Geo</t>
   </si>
   <si>
@@ -241,6 +229,12 @@
   </si>
   <si>
     <t>annual</t>
+  </si>
+  <si>
+    <t>get_mprop</t>
+  </si>
+  <si>
+    <t>get_wibrs</t>
   </si>
 </sst>
 </file>
@@ -597,7 +591,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,567 +634,567 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="K1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="N1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
       <c r="J2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M2" s="2">
         <v>38353</v>
       </c>
       <c r="N2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="K5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M5" s="2">
         <v>38895</v>
       </c>
       <c r="N5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M6" s="2">
         <v>43101</v>
       </c>
       <c r="N6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M7" s="2">
         <v>43101</v>
       </c>
       <c r="N7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="N9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M10" s="2">
         <v>41422</v>
       </c>
       <c r="N10" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M11" s="2">
         <v>40182</v>
       </c>
       <c r="N11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
         <v>55</v>
       </c>
-      <c r="B12" t="s">
-        <v>59</v>
-      </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="L12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="N12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="L13" t="s">
-        <v>64</v>
-      </c>
-      <c r="N13" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+      <c r="M13" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="L14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="M14">
         <v>2014</v>

</xml_diff>